<commit_message>
Dropped lines from plots.
</commit_message>
<xml_diff>
--- a/dat/Table2_ICU-beds-usage-QldVicNSW.xlsx
+++ b/dat/Table2_ICU-beds-usage-QldVicNSW.xlsx
@@ -140,14 +140,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,85 +434,85 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -520,7 +520,7 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>43918</v>
       </c>
       <c r="C3">
@@ -532,7 +532,7 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <f>SUM(C3:E3)</f>
         <v>3</v>
       </c>
@@ -545,7 +545,7 @@
       <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <f>SUM(G3:I3)</f>
         <v>34</v>
       </c>
@@ -558,7 +558,7 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <f>SUM(K3:M3)</f>
         <v>11</v>
       </c>
@@ -567,7 +567,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>43919</v>
       </c>
       <c r="C4">
@@ -579,8 +579,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" s="2">
-        <f t="shared" ref="F4:F8" si="0">SUM(C4:E4)</f>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F5" si="0">SUM(C4:E4)</f>
         <v>3</v>
       </c>
       <c r="G4">
@@ -592,8 +592,8 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J8" si="1">SUM(G4:I4)</f>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J7" si="1">SUM(G4:I4)</f>
         <v>43</v>
       </c>
       <c r="K4">
@@ -605,8 +605,8 @@
       <c r="M4">
         <v>0</v>
       </c>
-      <c r="N4" s="2">
-        <f t="shared" ref="N4:N8" si="2">SUM(K4:M4)</f>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N7" si="2">SUM(K4:M4)</f>
         <v>8</v>
       </c>
     </row>
@@ -614,7 +614,7 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>43920</v>
       </c>
       <c r="C5">
@@ -626,7 +626,7 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -639,7 +639,7 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
@@ -652,7 +652,7 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -661,7 +661,7 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>43921</v>
       </c>
     </row>
@@ -669,7 +669,7 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>43922</v>
       </c>
       <c r="G7">
@@ -681,7 +681,7 @@
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
@@ -691,7 +691,7 @@
       <c r="L7">
         <v>11</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>43923</v>
       </c>
     </row>

</xml_diff>